<commit_message>
some stuff re-written, model consult node working, TODOs and two nodes remaining
</commit_message>
<xml_diff>
--- a/models/DEModel_modified.xlsx
+++ b/models/DEModel_modified.xlsx
@@ -3717,10 +3717,11 @@
           <t>[2016 4.1;2030 4.1;2040 0]</t>
         </is>
       </c>
-      <c r="N34" s="5" t="inlineStr">
-        <is>
-          <t>[2016 4.1;2030 4.1;2040 0]</t>
-        </is>
+      <c r="M34" t="n">
+        <v>0</v>
+      </c>
+      <c r="N34" s="5" t="n">
+        <v>0</v>
       </c>
       <c r="O34" s="4" t="n"/>
       <c r="Q34" s="5" t="n">
@@ -3772,10 +3773,11 @@
         <v>0</v>
       </c>
       <c r="L35" s="5" t="n"/>
-      <c r="N35" s="5" t="inlineStr">
-        <is>
-          <t>[2016 0;2035 355]</t>
-        </is>
+      <c r="M35" t="n">
+        <v>0</v>
+      </c>
+      <c r="N35" s="5" t="n">
+        <v>0</v>
       </c>
       <c r="O35" s="4" t="n">
         <v>25</v>
@@ -3839,10 +3841,11 @@
           <t>[2016 45.4;2030 30;2040 0]</t>
         </is>
       </c>
-      <c r="N36" s="5" t="inlineStr">
-        <is>
-          <t>[2016 45.4;2030 30;2040 0]</t>
-        </is>
+      <c r="M36" t="n">
+        <v>0</v>
+      </c>
+      <c r="N36" s="5" t="n">
+        <v>0</v>
       </c>
       <c r="O36" s="4" t="n"/>
       <c r="Q36" s="5" t="n">
@@ -3894,10 +3897,11 @@
         <v>0</v>
       </c>
       <c r="L37" s="5" t="n"/>
-      <c r="N37" s="5" t="inlineStr">
-        <is>
-          <t>[2016 0;2035 180]</t>
-        </is>
+      <c r="M37" t="n">
+        <v>0</v>
+      </c>
+      <c r="N37" s="5" t="n">
+        <v>0</v>
       </c>
       <c r="O37" s="4" t="n">
         <v>25</v>
@@ -4909,7 +4913,7 @@
         <v>104</v>
       </c>
       <c r="R61" s="5" t="n">
-        <v>178.08</v>
+        <v>3500</v>
       </c>
       <c r="S61" s="4" t="n"/>
       <c r="T61" s="5" t="n"/>

</xml_diff>